<commit_message>
se modifico la tabla y se agregaron las CC
</commit_message>
<xml_diff>
--- a/TPsPrograDe4-master/Estadisticas.xlsx
+++ b/TPsPrograDe4-master/Estadisticas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baidab\Desktop\para pasar\unlam\Progra Avanzada\TPs Clase\TPsPrograDe4-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\TPsPrograDe4\TPsPrograDe4-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>ANALISIS DE RENDIMIENTO EN NS</t>
   </si>
@@ -52,12 +52,24 @@
   <si>
     <t>evaluarPow</t>
   </si>
+  <si>
+    <t>Complejidad Computacional</t>
+  </si>
+  <si>
+    <t>Algoritmo</t>
+  </si>
+  <si>
+    <t>n^2</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,8 +84,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,6 +103,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -172,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -195,9 +227,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,7 +255,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -236,22 +275,27 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-AR"/>
-              <a:t>Grafico de complejidades</a:t>
+              <a:rPr lang="es-419" sz="3200" b="1" u="none"/>
+              <a:t>Comparación</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="es-419" sz="3200" b="1" baseline="0"/>
+              <a:t> de rendimiento</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-419" sz="3200" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -269,25 +313,35 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10435099370088312"/>
+          <c:y val="0.11102278819120122"/>
+          <c:w val="0.89564903003304042"/>
+          <c:h val="0.78278066514211497"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -296,17 +350,17 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$A$3</c:f>
+              <c:f>Hoja1!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Grado de Polinomio</c:v>
+                  <c:v>evaluarProgDinamica</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -317,7 +371,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
               <c:f>Hoja1!$A$4:$A$11</c:f>
               <c:numCache>
@@ -349,25 +403,63 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$4:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>766799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>214800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1483200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1541700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1630200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>897300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>370600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>797700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B00E-4E71-848B-7240C07DBD6E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$3</c:f>
+              <c:f>Hoja1!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarProgDinamica</c:v>
+                  <c:v>evaluarMejorada</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -378,57 +470,95 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$4:$B$11</c:f>
+              <c:f>Hoja1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>63810</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73628</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53548</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67827</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49086</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103971</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>103079</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>172691</c:v>
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>596000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>156900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1236600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>808400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>453700</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>575600</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>295200</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>684200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B00E-4E71-848B-7240C07DBD6E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$3</c:f>
+              <c:f>Hoja1!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarMejorada</c:v>
+                  <c:v>evaluarMSucesivas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -439,57 +569,95 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$4:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$4:$C$11</c:f>
+              <c:f>Hoja1!$D$4:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>67827</c:v>
+                  <c:v>14735001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70951</c:v>
+                  <c:v>10563100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79875</c:v>
+                  <c:v>19693800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56225</c:v>
+                  <c:v>17202600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>67827</c:v>
+                  <c:v>54480300</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>82553</c:v>
+                  <c:v>12902900</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>132084</c:v>
+                  <c:v>18493700</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>124499</c:v>
+                  <c:v>31446500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B00E-4E71-848B-7240C07DBD6E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$D$3</c:f>
+              <c:f>Hoja1!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarMSucesivas</c:v>
+                  <c:v>evaluarRecursiva</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -500,57 +668,95 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$4:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$4:$D$11</c:f>
+              <c:f>Hoja1!$E$4:$E$11</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2049089</c:v>
+                  <c:v>597799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1890231</c:v>
+                  <c:v>215700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3370376</c:v>
+                  <c:v>2273100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1447571</c:v>
+                  <c:v>4209000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2980372</c:v>
+                  <c:v>4840800</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8863916</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>8479712</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>9225362</c:v>
+                  <c:v>5240000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8510100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13767000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B00E-4E71-848B-7240C07DBD6E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$3</c:f>
+              <c:f>Hoja1!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarRecursiva</c:v>
+                  <c:v>evaluarRecursivaPar</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
@@ -561,57 +767,95 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$E$4:$E$11</c:f>
+              <c:f>Hoja1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>80768</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>138777</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>454709</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>541278</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>974566</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3786709</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5908979</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10209746</c:v>
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$F$4:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>742700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>495900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3420100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2304900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6817300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4047700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6870800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15096100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B00E-4E71-848B-7240C07DBD6E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$F$3</c:f>
+              <c:f>Hoja1!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarRecursivaPar</c:v>
+                  <c:v>evaluarHorner</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
@@ -622,57 +866,95 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$F$4:$F$11</c:f>
+              <c:f>Hoja1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>53994</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76305</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98617</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>279340</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>406069</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2401611</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4565381</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9252136</c:v>
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$G$4:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>517300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>185700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>777800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>666800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1645000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>541100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>284900</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>370600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B00E-4E71-848B-7240C07DBD6E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$G$3</c:f>
+              <c:f>Hoja1!$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarHorner</c:v>
+                  <c:v>evaluarPow</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
@@ -685,69 +967,39 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$G$4:$G$11</c:f>
+              <c:f>Hoja1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>58902</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65596</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44177</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66488</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40161</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64257</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80768</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>91031</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja1!$H$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>evaluarPow</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Hoja1!$H$4:$H$11</c:f>
@@ -755,33 +1007,38 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>54440</c:v>
+                  <c:v>1921700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82107</c:v>
+                  <c:v>226700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88354</c:v>
+                  <c:v>990900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>174476</c:v>
+                  <c:v>906700</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>424365</c:v>
+                  <c:v>1732900</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2621602</c:v>
+                  <c:v>5358200</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5178501</c:v>
+                  <c:v>6339200</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9325318</c:v>
+                  <c:v>12956700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B00E-4E71-848B-7240C07DBD6E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -792,16 +1049,72 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="278804624"/>
-        <c:axId val="278803840"/>
+        <c:axId val="1555203743"/>
+        <c:axId val="1555197087"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="278804624"/>
+        <c:axId val="1555203743"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-419"/>
+                  <a:t>Grado</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-419"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -824,7 +1137,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -836,10 +1149,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278803840"/>
+        <c:crossAx val="1555197087"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -847,7 +1160,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="278803840"/>
+        <c:axId val="1555197087"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,6 +1180,76 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-419"/>
+                  <a:t>Tiempo en ns</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-419"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -895,10 +1278,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278804624"/>
+        <c:crossAx val="1555203743"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -938,7 +1321,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -968,7 +1351,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="es-419"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1020,7 +1403,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1031,7 +1414,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1054,14 +1437,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1077,7 +1460,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1097,22 +1480,17 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1121,12 +1499,12 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1136,12 +1514,12 @@
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1153,13 +1531,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="38100" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1168,36 +1546,29 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1219,15 +1590,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1242,15 +1611,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1261,17 +1630,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1280,14 +1649,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1299,21 +1668,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1332,7 +1695,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1351,17 +1714,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1370,17 +1733,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1401,7 +1763,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -1409,7 +1771,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1422,6 +1784,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1429,10 +1802,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1447,13 +1820,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
+    <cs:fontRef idx="major">
       <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1462,14 +1835,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1499,8 +1872,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1523,14 +1896,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1540,19 +1907,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:colOff>476252</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:rowOff>46462</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:colOff>639536</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="5" name="Gráfico 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1833,34 +2200,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1894,25 +2266,25 @@
         <v>5</v>
       </c>
       <c r="B4" s="4">
-        <v>63810</v>
+        <v>766799</v>
       </c>
       <c r="C4" s="5">
-        <v>67827</v>
+        <v>596000</v>
       </c>
       <c r="D4" s="5">
-        <v>2049089</v>
+        <v>14735001</v>
       </c>
       <c r="E4" s="4">
-        <v>80768</v>
+        <v>597799</v>
       </c>
       <c r="F4" s="4">
-        <v>53994</v>
+        <v>742700</v>
       </c>
       <c r="G4" s="4">
-        <v>58902</v>
+        <v>517300</v>
       </c>
       <c r="H4" s="4">
-        <v>54440</v>
+        <v>1921700</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1920,25 +2292,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="6">
-        <v>73628</v>
+        <v>214800</v>
       </c>
       <c r="C5" s="7">
-        <v>70951</v>
+        <v>156900</v>
       </c>
       <c r="D5" s="7">
-        <v>1890231</v>
+        <v>10563100</v>
       </c>
       <c r="E5" s="6">
-        <v>138777</v>
+        <v>215700</v>
       </c>
       <c r="F5" s="6">
-        <v>76305</v>
+        <v>495900</v>
       </c>
       <c r="G5" s="6">
-        <v>65596</v>
+        <v>185700</v>
       </c>
       <c r="H5" s="6">
-        <v>82107</v>
+        <v>226700</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1946,25 +2318,25 @@
         <v>100</v>
       </c>
       <c r="B6" s="6">
-        <v>53548</v>
+        <v>1483200</v>
       </c>
       <c r="C6" s="7">
-        <v>79875</v>
+        <v>1236600</v>
       </c>
       <c r="D6" s="7">
-        <v>3370376</v>
+        <v>19693800</v>
       </c>
       <c r="E6" s="6">
-        <v>454709</v>
+        <v>2273100</v>
       </c>
       <c r="F6" s="6">
-        <v>98617</v>
+        <v>3420100</v>
       </c>
       <c r="G6" s="6">
-        <v>44177</v>
+        <v>777800</v>
       </c>
       <c r="H6" s="6">
-        <v>88354</v>
+        <v>990900</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1972,25 +2344,25 @@
         <v>250</v>
       </c>
       <c r="B7" s="6">
-        <v>67827</v>
+        <v>1541700</v>
       </c>
       <c r="C7" s="7">
-        <v>56225</v>
+        <v>808400</v>
       </c>
       <c r="D7" s="7">
-        <v>1447571</v>
+        <v>17202600</v>
       </c>
       <c r="E7" s="6">
-        <v>541278</v>
+        <v>4209000</v>
       </c>
       <c r="F7" s="6">
-        <v>279340</v>
+        <v>2304900</v>
       </c>
       <c r="G7" s="6">
-        <v>66488</v>
+        <v>666800</v>
       </c>
       <c r="H7" s="6">
-        <v>174476</v>
+        <v>906700</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1998,25 +2370,25 @@
         <v>500</v>
       </c>
       <c r="B8" s="6">
-        <v>49086</v>
+        <v>1630200</v>
       </c>
       <c r="C8" s="7">
-        <v>67827</v>
+        <v>453700</v>
       </c>
       <c r="D8" s="7">
-        <v>2980372</v>
+        <v>54480300</v>
       </c>
       <c r="E8" s="6">
-        <v>974566</v>
+        <v>4840800</v>
       </c>
       <c r="F8" s="6">
-        <v>406069</v>
+        <v>6817300</v>
       </c>
       <c r="G8" s="6">
-        <v>40161</v>
+        <v>1645000</v>
       </c>
       <c r="H8" s="6">
-        <v>424365</v>
+        <v>1732900</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2024,25 +2396,25 @@
         <v>1000</v>
       </c>
       <c r="B9" s="6">
-        <v>103971</v>
+        <v>897300</v>
       </c>
       <c r="C9" s="7">
-        <v>82553</v>
+        <v>575600</v>
       </c>
       <c r="D9" s="7">
-        <v>8863916</v>
+        <v>12902900</v>
       </c>
       <c r="E9" s="6">
-        <v>3786709</v>
+        <v>5240000</v>
       </c>
       <c r="F9" s="6">
-        <v>2401611</v>
+        <v>4047700</v>
       </c>
       <c r="G9" s="6">
-        <v>64257</v>
+        <v>541100</v>
       </c>
       <c r="H9" s="6">
-        <v>2621602</v>
+        <v>5358200</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2050,25 +2422,25 @@
         <v>1500</v>
       </c>
       <c r="B10" s="6">
-        <v>103079</v>
+        <v>370600</v>
       </c>
       <c r="C10" s="6">
-        <v>132084</v>
+        <v>295200</v>
       </c>
       <c r="D10" s="6">
-        <v>8479712</v>
+        <v>18493700</v>
       </c>
       <c r="E10" s="6">
-        <v>5908979</v>
+        <v>8510100</v>
       </c>
       <c r="F10" s="6">
-        <v>4565381</v>
+        <v>6870800</v>
       </c>
       <c r="G10" s="6">
-        <v>80768</v>
+        <v>284900</v>
       </c>
       <c r="H10" s="6">
-        <v>5178501</v>
+        <v>6339200</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2076,32 +2448,101 @@
         <v>2000</v>
       </c>
       <c r="B11" s="6">
-        <v>172691</v>
+        <v>797700</v>
       </c>
       <c r="C11" s="6">
-        <v>124499</v>
+        <v>684200</v>
       </c>
       <c r="D11" s="6">
-        <v>9225362</v>
+        <v>31446500</v>
       </c>
       <c r="E11" s="6">
-        <v>10209746</v>
+        <v>13767000</v>
       </c>
       <c r="F11" s="6">
-        <v>9252136</v>
-      </c>
-      <c r="G11" s="6">
-        <v>91031</v>
+        <v>15096100</v>
+      </c>
+      <c r="G11" s="8">
+        <v>370600</v>
       </c>
       <c r="H11" s="6">
-        <v>9325318</v>
-      </c>
+        <v>12956700</v>
+      </c>
+    </row>
+    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F17" s="9"/>
+    </row>
+    <row r="19" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N19" s="9"/>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modificacion de las estadisticas
</commit_message>
<xml_diff>
--- a/TPsPrograDe4-master/Estadisticas.xlsx
+++ b/TPsPrograDe4-master/Estadisticas.xlsx
@@ -9,22 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>ANALISIS DE RENDIMIENTO EN NS</t>
   </si>
@@ -53,16 +59,25 @@
     <t>evaluarPow</t>
   </si>
   <si>
+    <t>Algoritmo</t>
+  </si>
+  <si>
     <t>Complejidad Computacional</t>
   </si>
   <si>
-    <t>Algoritmo</t>
+    <t>O(n)</t>
   </si>
   <si>
-    <t>n^2</t>
+    <t>O(n^2)</t>
   </si>
   <si>
-    <t>n</t>
+    <t>O(n*log n)</t>
+  </si>
+  <si>
+    <t>evaluarMsucesivas</t>
+  </si>
+  <si>
+    <t>evaluar Horner</t>
   </si>
 </sst>
 </file>
@@ -102,12 +117,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -118,71 +127,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -200,43 +157,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -275,27 +254,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mj-lt"/>
-                <a:ea typeface="+mj-ea"/>
-                <a:cs typeface="+mj-cs"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-419" sz="3200" b="1" u="none"/>
-              <a:t>Comparación</a:t>
+              <a:rPr lang="es-419"/>
+              <a:t>Comparación de algoritmos</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="es-419" sz="3200" b="1" baseline="0"/>
-              <a:t> de rendimiento</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-419" sz="3200" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -313,16 +287,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="es-419"/>
@@ -331,17 +305,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.10435099370088312"/>
-          <c:y val="0.11102278819120122"/>
-          <c:w val="0.89564903003304042"/>
-          <c:h val="0.78278066514211497"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -354,13 +318,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarProgDinamica</c:v>
+                  <c:v>evaluarMsucesivas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -369,7 +333,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -411,28 +387,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>766799</c:v>
+                  <c:v>2911334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>214800</c:v>
+                  <c:v>3445689</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1483200</c:v>
+                  <c:v>3420267</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1541700</c:v>
+                  <c:v>3529778</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1630200</c:v>
+                  <c:v>5522490</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>897300</c:v>
+                  <c:v>6140445</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>370600</c:v>
+                  <c:v>5679912</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>797700</c:v>
+                  <c:v>7611512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -440,7 +416,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B00E-4E71-848B-7240C07DBD6E}"/>
+              <c16:uniqueId val="{00000008-8002-4417-85A7-AE2EA7EF89BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -453,13 +429,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarMejorada</c:v>
+                  <c:v>evaluarRecursiva</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -468,7 +444,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -507,31 +495,31 @@
             <c:numRef>
               <c:f>Hoja1!$C$4:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>596000</c:v>
+                  <c:v>98756</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156900</c:v>
+                  <c:v>68444</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1236600</c:v>
+                  <c:v>621377</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>808400</c:v>
+                  <c:v>925956</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>453700</c:v>
+                  <c:v>1655378</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>575600</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>295200</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>684200</c:v>
+                  <c:v>2790578</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5688712</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9297690</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -539,7 +527,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B00E-4E71-848B-7240C07DBD6E}"/>
+              <c16:uniqueId val="{00000009-8002-4417-85A7-AE2EA7EF89BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -552,13 +540,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarMSucesivas</c:v>
+                  <c:v>evaluarRecursivaPar</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -567,7 +555,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -606,31 +606,31 @@
             <c:numRef>
               <c:f>Hoja1!$D$4:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>14735001</c:v>
+                  <c:v>207289</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10563100</c:v>
+                  <c:v>55244</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19693800</c:v>
+                  <c:v>269377</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17202600</c:v>
+                  <c:v>323645</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54480300</c:v>
+                  <c:v>747022</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12902900</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>18493700</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>31446500</c:v>
+                  <c:v>2215645</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4708978</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8240223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -638,7 +638,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B00E-4E71-848B-7240C07DBD6E}"/>
+              <c16:uniqueId val="{0000000A-8002-4417-85A7-AE2EA7EF89BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -651,13 +651,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarRecursiva</c:v>
+                  <c:v>evaluarProgDinamica</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -666,7 +666,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -708,28 +720,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>597799</c:v>
+                  <c:v>55244</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>215700</c:v>
+                  <c:v>53777</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2273100</c:v>
+                  <c:v>158400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4209000</c:v>
+                  <c:v>165734</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4840800</c:v>
+                  <c:v>182844</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5240000</c:v>
+                  <c:v>260088</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8510100</c:v>
+                  <c:v>121244</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13767000</c:v>
+                  <c:v>132489</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -737,7 +749,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-B00E-4E71-848B-7240C07DBD6E}"/>
+              <c16:uniqueId val="{0000000B-8002-4417-85A7-AE2EA7EF89BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -750,13 +762,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarRecursivaPar</c:v>
+                  <c:v>evaluarMejorada</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
@@ -765,7 +777,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -807,28 +831,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>742700</c:v>
+                  <c:v>56222</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>495900</c:v>
+                  <c:v>50845</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3420100</c:v>
+                  <c:v>170622</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2304900</c:v>
+                  <c:v>147156</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6817300</c:v>
+                  <c:v>183334</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4047700</c:v>
+                  <c:v>216089</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6870800</c:v>
+                  <c:v>99244</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15096100</c:v>
+                  <c:v>114889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -836,7 +860,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-B00E-4E71-848B-7240C07DBD6E}"/>
+              <c16:uniqueId val="{0000000C-8002-4417-85A7-AE2EA7EF89BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -849,13 +873,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarHorner</c:v>
+                  <c:v>evaluarPow</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
@@ -864,7 +888,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -906,28 +942,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>517300</c:v>
+                  <c:v>51822</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>185700</c:v>
+                  <c:v>49378</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>777800</c:v>
+                  <c:v>154000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>666800</c:v>
+                  <c:v>257644</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1645000</c:v>
+                  <c:v>727467</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>541100</c:v>
+                  <c:v>2702578</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>284900</c:v>
+                  <c:v>4767157</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>370600</c:v>
+                  <c:v>8923690</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -935,7 +971,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-B00E-4E71-848B-7240C07DBD6E}"/>
+              <c16:uniqueId val="{0000000D-8002-4417-85A7-AE2EA7EF89BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -948,13 +984,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>evaluarPow</c:v>
+                  <c:v>evaluar Horner</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
@@ -965,7 +1001,23 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1007,28 +1059,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1921700</c:v>
+                  <c:v>48888</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>226700</c:v>
+                  <c:v>47422</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>990900</c:v>
+                  <c:v>120266</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>906700</c:v>
+                  <c:v>131511</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1732900</c:v>
+                  <c:v>137378</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5358200</c:v>
+                  <c:v>209245</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6339200</c:v>
+                  <c:v>71378</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12956700</c:v>
+                  <c:v>90445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1036,7 +1088,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-B00E-4E71-848B-7240C07DBD6E}"/>
+              <c16:uniqueId val="{0000000E-8002-4417-85A7-AE2EA7EF89BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1048,73 +1100,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1555203743"/>
-        <c:axId val="1555197087"/>
+        <c:axId val="1400186399"/>
+        <c:axId val="1400180991"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1555203743"/>
+        <c:axId val="1400186399"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="es-419"/>
-                  <a:t>Grado</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-419"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1137,7 +1134,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1152,7 +1149,7 @@
             <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1555197087"/>
+        <c:crossAx val="1400180991"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1160,7 +1157,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1555197087"/>
+        <c:axId val="1400180991"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,76 +1177,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="es-419"/>
-                  <a:t>Tiempo en ns</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-419"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1281,7 +1208,7 @@
             <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1555203743"/>
+        <c:crossAx val="1400186399"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1403,7 +1330,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1414,7 +1341,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1437,14 +1364,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1460,7 +1387,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1480,17 +1407,22 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1499,45 +1431,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="38100" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1546,29 +1468,33 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1590,13 +1516,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1611,15 +1539,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1630,17 +1558,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1649,14 +1577,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1668,15 +1596,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1695,7 +1629,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1714,17 +1648,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1733,16 +1667,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1763,7 +1698,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -1771,7 +1706,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1784,17 +1719,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1802,10 +1726,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1820,13 +1744,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1835,14 +1759,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1872,8 +1796,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1896,8 +1820,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1906,20 +1836,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>476252</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>46462</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38877</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>639536</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>231711</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>115077</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Gráfico 4"/>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2200,21 +2130,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D4" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
@@ -2234,313 +2165,324 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="8" t="s">
         <v>8</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>766799</v>
+      <c r="B4" s="5">
+        <v>2911334</v>
       </c>
       <c r="C4" s="5">
-        <v>596000</v>
+        <v>98756</v>
       </c>
       <c r="D4" s="5">
-        <v>14735001</v>
-      </c>
-      <c r="E4" s="4">
-        <v>597799</v>
-      </c>
-      <c r="F4" s="4">
-        <v>742700</v>
-      </c>
-      <c r="G4" s="4">
-        <v>517300</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1921700</v>
+        <v>207289</v>
+      </c>
+      <c r="E4" s="5">
+        <v>55244</v>
+      </c>
+      <c r="F4" s="5">
+        <v>56222</v>
+      </c>
+      <c r="G4" s="5">
+        <v>51822</v>
+      </c>
+      <c r="H4" s="5">
+        <v>48888</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>10</v>
       </c>
-      <c r="B5" s="6">
-        <v>214800</v>
-      </c>
-      <c r="C5" s="7">
-        <v>156900</v>
-      </c>
-      <c r="D5" s="7">
-        <v>10563100</v>
-      </c>
-      <c r="E5" s="6">
-        <v>215700</v>
-      </c>
-      <c r="F5" s="6">
-        <v>495900</v>
-      </c>
-      <c r="G5" s="6">
-        <v>185700</v>
-      </c>
-      <c r="H5" s="6">
-        <v>226700</v>
+      <c r="B5" s="5">
+        <v>3445689</v>
+      </c>
+      <c r="C5" s="5">
+        <v>68444</v>
+      </c>
+      <c r="D5" s="5">
+        <v>55244</v>
+      </c>
+      <c r="E5" s="5">
+        <v>53777</v>
+      </c>
+      <c r="F5" s="5">
+        <v>50845</v>
+      </c>
+      <c r="G5" s="5">
+        <v>49378</v>
+      </c>
+      <c r="H5" s="5">
+        <v>47422</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>100</v>
       </c>
-      <c r="B6" s="6">
-        <v>1483200</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1236600</v>
-      </c>
-      <c r="D6" s="7">
-        <v>19693800</v>
-      </c>
-      <c r="E6" s="6">
-        <v>2273100</v>
-      </c>
-      <c r="F6" s="6">
-        <v>3420100</v>
-      </c>
-      <c r="G6" s="6">
-        <v>777800</v>
-      </c>
-      <c r="H6" s="6">
-        <v>990900</v>
+      <c r="B6" s="5">
+        <v>3420267</v>
+      </c>
+      <c r="C6" s="5">
+        <v>621377</v>
+      </c>
+      <c r="D6" s="5">
+        <v>269377</v>
+      </c>
+      <c r="E6" s="5">
+        <v>158400</v>
+      </c>
+      <c r="F6" s="5">
+        <v>170622</v>
+      </c>
+      <c r="G6" s="5">
+        <v>154000</v>
+      </c>
+      <c r="H6" s="5">
+        <v>120266</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>250</v>
       </c>
-      <c r="B7" s="6">
-        <v>1541700</v>
-      </c>
-      <c r="C7" s="7">
-        <v>808400</v>
-      </c>
-      <c r="D7" s="7">
-        <v>17202600</v>
-      </c>
-      <c r="E7" s="6">
-        <v>4209000</v>
-      </c>
-      <c r="F7" s="6">
-        <v>2304900</v>
-      </c>
-      <c r="G7" s="6">
-        <v>666800</v>
-      </c>
-      <c r="H7" s="6">
-        <v>906700</v>
+      <c r="B7" s="5">
+        <v>3529778</v>
+      </c>
+      <c r="C7" s="5">
+        <v>925956</v>
+      </c>
+      <c r="D7" s="5">
+        <v>323645</v>
+      </c>
+      <c r="E7" s="5">
+        <v>165734</v>
+      </c>
+      <c r="F7" s="5">
+        <v>147156</v>
+      </c>
+      <c r="G7" s="5">
+        <v>257644</v>
+      </c>
+      <c r="H7" s="5">
+        <v>131511</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>500</v>
       </c>
-      <c r="B8" s="6">
-        <v>1630200</v>
-      </c>
-      <c r="C8" s="7">
-        <v>453700</v>
-      </c>
-      <c r="D8" s="7">
-        <v>54480300</v>
-      </c>
-      <c r="E8" s="6">
-        <v>4840800</v>
-      </c>
-      <c r="F8" s="6">
-        <v>6817300</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1645000</v>
+      <c r="B8" s="5">
+        <v>5522490</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1655378</v>
+      </c>
+      <c r="D8" s="5">
+        <v>747022</v>
+      </c>
+      <c r="E8" s="5">
+        <v>182844</v>
+      </c>
+      <c r="F8" s="5">
+        <v>183334</v>
+      </c>
+      <c r="G8" s="5">
+        <v>727467</v>
       </c>
       <c r="H8" s="6">
-        <v>1732900</v>
+        <v>137378</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>1000</v>
       </c>
-      <c r="B9" s="6">
-        <v>897300</v>
-      </c>
-      <c r="C9" s="7">
-        <v>575600</v>
-      </c>
-      <c r="D9" s="7">
-        <v>12902900</v>
-      </c>
-      <c r="E9" s="6">
-        <v>5240000</v>
-      </c>
-      <c r="F9" s="6">
-        <v>4047700</v>
-      </c>
-      <c r="G9" s="6">
-        <v>541100</v>
-      </c>
-      <c r="H9" s="6">
-        <v>5358200</v>
+      <c r="B9" s="5">
+        <v>6140445</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2790578</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2215645</v>
+      </c>
+      <c r="E9" s="5">
+        <v>260088</v>
+      </c>
+      <c r="F9" s="5">
+        <v>216089</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2702578</v>
+      </c>
+      <c r="H9" s="5">
+        <v>209245</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>1500</v>
       </c>
-      <c r="B10" s="6">
-        <v>370600</v>
-      </c>
-      <c r="C10" s="6">
-        <v>295200</v>
-      </c>
-      <c r="D10" s="6">
-        <v>18493700</v>
-      </c>
-      <c r="E10" s="6">
-        <v>8510100</v>
-      </c>
-      <c r="F10" s="6">
-        <v>6870800</v>
-      </c>
-      <c r="G10" s="6">
-        <v>284900</v>
-      </c>
-      <c r="H10" s="6">
-        <v>6339200</v>
+      <c r="B10" s="5">
+        <v>5679912</v>
+      </c>
+      <c r="C10" s="5">
+        <v>5688712</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4708978</v>
+      </c>
+      <c r="E10" s="5">
+        <v>121244</v>
+      </c>
+      <c r="F10" s="5">
+        <v>99244</v>
+      </c>
+      <c r="G10" s="5">
+        <v>4767157</v>
+      </c>
+      <c r="H10" s="5">
+        <v>71378</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>2000</v>
       </c>
-      <c r="B11" s="6">
-        <v>797700</v>
-      </c>
-      <c r="C11" s="6">
-        <v>684200</v>
-      </c>
-      <c r="D11" s="6">
-        <v>31446500</v>
-      </c>
-      <c r="E11" s="6">
-        <v>13767000</v>
-      </c>
-      <c r="F11" s="6">
-        <v>15096100</v>
-      </c>
-      <c r="G11" s="8">
-        <v>370600</v>
-      </c>
-      <c r="H11" s="6">
-        <v>12956700</v>
+      <c r="B11" s="5">
+        <v>7611512</v>
+      </c>
+      <c r="C11" s="5">
+        <v>9297690</v>
+      </c>
+      <c r="D11" s="5">
+        <v>8240223</v>
+      </c>
+      <c r="E11" s="5">
+        <v>132489</v>
+      </c>
+      <c r="F11" s="5">
+        <v>114889</v>
+      </c>
+      <c r="G11" s="5">
+        <v>8923690</v>
+      </c>
+      <c r="H11" s="5">
+        <v>90445</v>
       </c>
     </row>
-    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F17" s="9"/>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
     </row>
-    <row r="19" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="N19" s="9"/>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N19" s="1"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="12" t="s">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="12" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="13" t="s">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>12</v>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="11" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>12</v>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="13" t="s">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="11"/>
+      <c r="C35" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
+  <conditionalFormatting sqref="A3:H3">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>